<commit_message>
add valores no mysql
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2301,6 +2301,21 @@
         </is>
       </c>
     </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>90711124</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>Kit Vaso Sanitário com Caixa Acoplada e Assento Branco Duplo Acionamento 3/6L Saída Vertical Vougan Docol</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>3.299.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
criando novos arquivos para organizar
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2316,6 +2316,81 @@
         </is>
       </c>
     </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>89521985</v>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>Trena Laser 40m GLM 40 Bosch</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>399.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>91093191</v>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Trena Laser 50m DW0165N Dewalt</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>529.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>91812875</v>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Esquadro Carpinteiro 12" Dexter</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>33.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>90525582</v>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>Óculos de Visualização Laser Bosch</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>47.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>1571028193</v>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Máscara Protetor Facial - Proteção Transparente</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>10.00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
====PROXIMO FILE TEM 'VENV'====
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C116"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2391,6 +2391,66 @@
         </is>
       </c>
     </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>89716123</v>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>Jogo de Ferramentas 108 peças em Aço Cromo Vanádio Dexter</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>499.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>1567614963</v>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Luva Vinil C/po G 100un/box Vabene</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>104.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>1567065435</v>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Protetor De Ouvido Equipamento De Segurança Abafador Som E Ruidos</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>77.90</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>90656125</v>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Óculos Anti-Embassamento Cayman Incolor Carbrografite</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>31.90</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
faendo teste só pra né
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2451,6 +2451,21 @@
         </is>
       </c>
     </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>90909903</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Persiana Blackout Rolô Belem Granito 2,20x2,20m Inspire</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>489.90</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
alterando no format data para float o preco
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2466,6 +2466,62 @@
         </is>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>1567227175</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Abraçadeiras De Nylon Para Lacre Brancas 7 6mm X 500mm</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>79.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>89801243</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Máquina de Pintura Elétrica 900W Airless MPA 120 220V Vonder</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>2.399.00</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>90795621</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Furadeira e Parafusadeira de Impacto a Bateria Bosch com Carregador e Bateria 18V 1/2" GSB 180-Li Bivolt</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>619.9</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>89837055</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Carvão Briquete 2,5Kg Pérola Negra</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>18.29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
trocando o salvamento em csv para um buffer
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C125"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2522,6 +2522,32 @@
         <v>18.29</v>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>92007776</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Jogo de Brocas para Metal e Madeira 19 Peças Dexter</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>89235783</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Luva Nylon Látex Maxigrip Pro M Danny</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>17.49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>

<commit_message>
Update format_values and search_data modules
</commit_message>
<xml_diff>
--- a/teste.xlsx
+++ b/teste.xlsx
@@ -421,7 +421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
@@ -2548,6 +2548,136 @@
         <v>17.49</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>92007895</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Jogo de Brocas Talhadeira e Ponteiro para Concreto SDS 6 Peças Dexter</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>49.9</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>92007762</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Jogo de Brocas com 5 para Madeira 6 para Metal e 5 para Alvenaria 16 Peças Dexter</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>89833870</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Jogo de Brocas de Vídea encaixe SDS Plus para Concreto 6 a 12mm 5 Peças Dexter</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>58.9</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>88162186</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Lixeira para Banheiro 3L Metal Aço Pedal Prata Escovado Sensea</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>89408333</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Sacos de Lixo Azul 50L Contém 50 Sacos Embalixo</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>19.79</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>89408270</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Sacos de Lixo Branco Pia e Banheiro Contém 100 Sacos 38x40cm Embalixo</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>19.79</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>90672694</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Saco Lixo Embalixo 100L Wecycle Reforçado Azul Com 10 Sacos</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>19.79</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>90672680</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Saco Lixo Embalixo 50L Reforçado Preto Com 50 Sacos</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>59.9</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>88187246</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Cabo de Aluminio 1,50m Bettanin</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>52.9</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>90351765</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Martelete Perfurador Rompedor Makita com Maleta com 5 Brocas e Acessórios SDS Plus 800W 2,7J HR 2470 220V</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>769.9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>

</xml_diff>